<commit_message>
Fix sheet name in test data `input.xlsx`
</commit_message>
<xml_diff>
--- a/src/test/resources/xls-import-multi/input.xlsx
+++ b/src/test/resources/xls-import-multi/input.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpra/Workspaces/gradle-android-i18n/gradle-android-i18n/src/test/resources/xls-import-multi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB362E4-1880-744E-8311-980866BFCFDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41071518-2C5D-DE41-A9EC-EC0F729E0092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app" sheetId="1" r:id="rId1"/>
-    <sheet name="features-feature1" sheetId="2" r:id="rId2"/>
+    <sheet name="features.feature-one" sheetId="2" r:id="rId2"/>
     <sheet name="lib" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -246,9 +246,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -267,6 +264,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -659,200 +659,200 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="2"/>
+    <col min="1" max="1" width="21.33203125" style="1"/>
     <col min="2" max="2" width="42"/>
     <col min="3" max="3" width="35.83203125"/>
     <col min="4" max="4" width="40.33203125"/>
     <col min="5" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -871,58 +871,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="2"/>
+    <col min="1" max="1" width="21.33203125" style="1"/>
     <col min="2" max="2" width="42"/>
     <col min="3" max="3" width="35.83203125"/>
     <col min="4" max="4" width="40.33203125"/>
     <col min="5" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -939,72 +939,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="2"/>
+    <col min="1" max="1" width="21.33203125" style="1"/>
     <col min="2" max="2" width="42"/>
     <col min="3" max="3" width="35.83203125"/>
     <col min="4" max="4" width="40.33203125"/>
     <col min="5" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>